<commit_message>
Multimetro  - Versão 100% final
- pdf incluido
- corrigir numeros de resistências e nomes de circuitos
</commit_message>
<xml_diff>
--- a/T2A-Multimetro.xlsx
+++ b/T2A-Multimetro.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sergi\OneDrive - Universidade do Porto\Ambiente de Trabalho\GIT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nunop\OneDrive\Documentos\GitHub\LABSFISICAI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B06CD92-2A61-41B5-BA5E-852E261F3FD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B0C0083-FCB4-4342-A413-F105262D7516}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{CF471F3A-E1A0-4176-A48E-87D105974DFD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CF471F3A-E1A0-4176-A48E-87D105974DFD}"/>
   </bookViews>
   <sheets>
     <sheet name="R1 CA" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="40">
   <si>
     <t>Numero de Medição</t>
   </si>
@@ -77,15 +77,6 @@
   </si>
   <si>
     <t>Incerteza na Média</t>
-  </si>
-  <si>
-    <t>Ciruito A Resistência 2</t>
-  </si>
-  <si>
-    <t>Ciruito A Resistência 1</t>
-  </si>
-  <si>
-    <t>Ciruito A Resistência 3</t>
   </si>
   <si>
     <t>V (V)</t>
@@ -222,6 +213,24 @@
       </rPr>
       <t>):</t>
     </r>
+  </si>
+  <si>
+    <t>Montagem 1 Resistência 4A</t>
+  </si>
+  <si>
+    <t>Montagem 2 Resistência 4B</t>
+  </si>
+  <si>
+    <t>Montagem 1 Resistência 4C</t>
+  </si>
+  <si>
+    <t>Montagem 1 Resistência 4B</t>
+  </si>
+  <si>
+    <t>Montagem 2 Resistência 4A</t>
+  </si>
+  <si>
+    <t>Montagem 2 Resistência 4C</t>
   </si>
 </sst>
 </file>
@@ -468,29 +477,17 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -516,20 +513,32 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -542,9 +551,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Moeda" xfId="1" builtinId="4"/>
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percentagem" xfId="2" builtinId="5"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="95">
     <dxf>
@@ -926,7 +935,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pt-PT"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -993,7 +1002,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-PT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1086,7 +1095,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="pt-PT"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1296,7 +1305,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="pt-PT"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1334,7 +1343,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="838937568"/>
@@ -1420,7 +1429,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="pt-PT"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1458,7 +1467,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="838931744"/>
@@ -1510,7 +1519,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-PT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1547,7 +1556,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="pt-PT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1561,7 +1570,7 @@
 <file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pt-PT"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1598,7 +1607,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-PT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1852,7 +1861,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="pt-PT"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1890,7 +1899,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1459642992"/>
@@ -1969,7 +1978,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="pt-PT"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2007,7 +2016,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1459645904"/>
@@ -2059,7 +2068,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-PT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2096,7 +2105,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="pt-PT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2110,7 +2119,7 @@
 <file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pt-PT"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2177,7 +2186,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-PT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2270,7 +2279,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="pt-PT"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -2480,7 +2489,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="pt-PT"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2518,7 +2527,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="838937568"/>
@@ -2604,7 +2613,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="pt-PT"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2642,7 +2651,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="838931744"/>
@@ -2694,7 +2703,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-PT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2731,7 +2740,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="pt-PT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2745,7 +2754,7 @@
 <file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pt-PT"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2782,7 +2791,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-PT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3011,7 +3020,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="pt-PT"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3049,7 +3058,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1459642992"/>
@@ -3103,7 +3112,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="pt-PT"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3141,7 +3150,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1459645904"/>
@@ -3193,7 +3202,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-PT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3230,7 +3239,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="pt-PT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3244,7 +3253,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pt-PT"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3281,7 +3290,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-PT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3534,7 +3543,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="pt-PT"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3572,7 +3581,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1459642992"/>
@@ -3651,7 +3660,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="pt-PT"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3689,7 +3698,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1459645904"/>
@@ -3741,7 +3750,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-PT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3778,7 +3787,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="pt-PT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3792,7 +3801,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pt-PT"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3859,7 +3868,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-PT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3952,7 +3961,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="pt-PT"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -4162,7 +4171,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="pt-PT"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4200,7 +4209,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="838937568"/>
@@ -4286,7 +4295,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="pt-PT"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4324,7 +4333,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="838931744"/>
@@ -4376,7 +4385,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-PT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4413,7 +4422,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="pt-PT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4427,7 +4436,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pt-PT"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -4464,7 +4473,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-PT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -4718,7 +4727,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="pt-PT"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4756,7 +4765,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1459642992"/>
@@ -4835,7 +4844,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="pt-PT"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4873,7 +4882,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1459645904"/>
@@ -4925,7 +4934,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-PT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4962,7 +4971,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="pt-PT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4976,7 +4985,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pt-PT"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -5043,7 +5052,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-PT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -5136,7 +5145,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="pt-PT"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -5346,7 +5355,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="pt-PT"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -5384,7 +5393,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="838937568"/>
@@ -5470,7 +5479,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="pt-PT"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -5508,7 +5517,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="838931744"/>
@@ -5560,7 +5569,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-PT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -5597,7 +5606,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="pt-PT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -5611,7 +5620,7 @@
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pt-PT"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -5648,7 +5657,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-PT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -5901,7 +5910,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="pt-PT"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -5939,7 +5948,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1459642992"/>
@@ -6018,7 +6027,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="pt-PT"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -6056,7 +6065,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1459645904"/>
@@ -6108,7 +6117,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-PT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -6145,7 +6154,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="pt-PT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -6159,7 +6168,7 @@
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pt-PT"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -6226,7 +6235,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-PT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -6319,7 +6328,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="pt-PT"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -6529,7 +6538,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="pt-PT"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -6567,7 +6576,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="838937568"/>
@@ -6653,7 +6662,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="pt-PT"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -6691,7 +6700,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="838931744"/>
@@ -6743,7 +6752,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-PT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -6780,7 +6789,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="pt-PT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -6794,7 +6803,7 @@
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pt-PT"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -6831,7 +6840,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-PT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -7083,7 +7092,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="pt-PT"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -7121,7 +7130,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1459642992"/>
@@ -7200,7 +7209,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="pt-PT"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -7238,7 +7247,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1459645904"/>
@@ -7290,7 +7299,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-PT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -7327,7 +7336,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="pt-PT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -7341,7 +7350,7 @@
 <file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pt-PT"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -7408,7 +7417,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-PT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -7501,7 +7510,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="pt-PT"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -7711,7 +7720,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="pt-PT"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -7749,7 +7758,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="838937568"/>
@@ -7835,7 +7844,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="pt-PT"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -7873,7 +7882,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="838931744"/>
@@ -7925,7 +7934,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-PT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -7962,7 +7971,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="pt-PT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -15266,7 +15275,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -15589,8 +15598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C93CEA2-7506-43DA-BD0E-18E2DA668FCC}">
   <dimension ref="A2:Y161"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15612,47 +15621,47 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A2" s="37" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
+      <c r="A2" s="47" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="E3" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>12</v>
-      </c>
       <c r="G3" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="1"/>
-      <c r="J3" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="K3" s="32"/>
+      <c r="K3" s="48"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" s="28">
@@ -15690,10 +15699,10 @@
       <c r="K4" s="22">
         <v>1.0668107153187556E-2</v>
       </c>
-      <c r="M4" s="49" t="s">
-        <v>33</v>
-      </c>
-      <c r="N4" s="49"/>
+      <c r="M4" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="N4" s="33"/>
     </row>
     <row r="5" spans="1:24" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="28">
@@ -15730,8 +15739,8 @@
       <c r="K5" s="22">
         <v>4.8452268459604148E-3</v>
       </c>
-      <c r="M5" s="49"/>
-      <c r="N5" s="49"/>
+      <c r="M5" s="33"/>
+      <c r="N5" s="33"/>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" s="28">
@@ -15768,8 +15777,8 @@
       <c r="K6" s="22">
         <v>8.8662934058695349E-3</v>
       </c>
-      <c r="M6" s="49"/>
-      <c r="N6" s="49"/>
+      <c r="M6" s="33"/>
+      <c r="N6" s="33"/>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" s="28">
@@ -15807,8 +15816,8 @@
         <v>13</v>
       </c>
       <c r="L7" s="1"/>
-      <c r="M7" s="49"/>
-      <c r="N7" s="49"/>
+      <c r="M7" s="33"/>
+      <c r="N7" s="33"/>
       <c r="O7" s="3"/>
       <c r="P7" s="17"/>
       <c r="Q7" s="3"/>
@@ -15919,15 +15928,15 @@
         <v>-2.5887254142547E-3</v>
       </c>
       <c r="I10" s="1"/>
-      <c r="J10" s="33" t="s">
+      <c r="J10" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="K10" s="34"/>
-      <c r="L10" s="35"/>
-      <c r="M10" s="47">
+      <c r="K10" s="44"/>
+      <c r="L10" s="45"/>
+      <c r="M10" s="30">
         <v>0.01</v>
       </c>
-      <c r="N10" s="47"/>
+      <c r="N10" s="30"/>
       <c r="R10" s="20"/>
       <c r="S10" s="20"/>
       <c r="T10" s="20"/>
@@ -15961,15 +15970,15 @@
         <v>2.5497777851284376E-3</v>
       </c>
       <c r="I11" s="1"/>
-      <c r="J11" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="K11" s="34"/>
-      <c r="L11" s="35"/>
-      <c r="M11" s="47">
+      <c r="J11" s="43" t="s">
+        <v>11</v>
+      </c>
+      <c r="K11" s="44"/>
+      <c r="L11" s="45"/>
+      <c r="M11" s="30">
         <v>9.9999999999999995E-8</v>
       </c>
-      <c r="N11" s="47"/>
+      <c r="N11" s="30"/>
       <c r="R11" s="20"/>
       <c r="S11" s="20"/>
       <c r="T11" s="20"/>
@@ -16003,15 +16012,15 @@
         <v>-1.5432937866028063E-2</v>
       </c>
       <c r="I12" s="1"/>
-      <c r="J12" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="K12" s="34"/>
-      <c r="L12" s="35"/>
-      <c r="M12" s="46">
+      <c r="J12" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="K12" s="44"/>
+      <c r="L12" s="45"/>
+      <c r="M12" s="31">
         <v>470</v>
       </c>
-      <c r="N12" s="46"/>
+      <c r="N12" s="31"/>
       <c r="R12" s="20"/>
       <c r="S12" s="20"/>
       <c r="T12" s="20"/>
@@ -16067,7 +16076,7 @@
         <v>1.1560000000000001E-2</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F14" s="5">
         <f t="shared" si="0"/>
@@ -16082,16 +16091,16 @@
         <v>1.961530158128344E-2</v>
       </c>
       <c r="I14" s="1"/>
-      <c r="J14" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="K14" s="34"/>
-      <c r="L14" s="35"/>
-      <c r="M14" s="46">
+      <c r="J14" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="K14" s="44"/>
+      <c r="L14" s="45"/>
+      <c r="M14" s="31">
         <f>J4</f>
         <v>465.37340754892119</v>
       </c>
-      <c r="N14" s="46"/>
+      <c r="N14" s="31"/>
       <c r="R14" s="20"/>
       <c r="S14" s="20"/>
       <c r="T14" s="20"/>
@@ -16125,16 +16134,16 @@
         <v>-1.6250279227154607E-3</v>
       </c>
       <c r="I15" s="1"/>
-      <c r="J15" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="K15" s="34"/>
-      <c r="L15" s="35"/>
-      <c r="M15" s="48">
+      <c r="J15" s="43" t="s">
+        <v>31</v>
+      </c>
+      <c r="K15" s="44"/>
+      <c r="L15" s="45"/>
+      <c r="M15" s="32">
         <f>J5</f>
         <v>0.50404609178452187</v>
       </c>
-      <c r="N15" s="48"/>
+      <c r="N15" s="32"/>
       <c r="R15" s="20"/>
       <c r="S15" s="20"/>
       <c r="T15" s="20"/>
@@ -16153,7 +16162,7 @@
         <v>1.3806000000000001E-2</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F16" s="5">
         <f t="shared" si="0"/>
@@ -16168,16 +16177,16 @@
         <v>-5.6133717735944444E-3</v>
       </c>
       <c r="I16" s="1"/>
-      <c r="J16" s="32" t="s">
-        <v>35</v>
-      </c>
-      <c r="K16" s="32"/>
-      <c r="L16" s="32"/>
-      <c r="M16" s="46">
+      <c r="J16" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="K16" s="48"/>
+      <c r="L16" s="48"/>
+      <c r="M16" s="31">
         <f>F20</f>
         <v>467.27349049454619</v>
       </c>
-      <c r="N16" s="46"/>
+      <c r="N16" s="31"/>
       <c r="R16" s="20"/>
       <c r="S16" s="20"/>
       <c r="T16" s="20"/>
@@ -16196,7 +16205,7 @@
         <v>1.4873000000000001E-2</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F17" s="5">
         <f t="shared" si="0"/>
@@ -16211,16 +16220,16 @@
         <v>-2.1667976282930823E-3</v>
       </c>
       <c r="I17" s="1"/>
-      <c r="J17" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="K17" s="30"/>
-      <c r="L17" s="30"/>
-      <c r="M17" s="48">
+      <c r="J17" s="46" t="s">
+        <v>21</v>
+      </c>
+      <c r="K17" s="46"/>
+      <c r="L17" s="46"/>
+      <c r="M17" s="32">
         <f>SQRT(((1/D20)*B22)^2+(-(B20/(D20^2))*D22)^2)</f>
         <v>115.64457411168775</v>
       </c>
-      <c r="N17" s="48"/>
+      <c r="N17" s="32"/>
       <c r="R17" s="20"/>
       <c r="S17" s="20"/>
       <c r="T17" s="20"/>
@@ -16264,16 +16273,16 @@
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-      <c r="J19" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="K19" s="36"/>
-      <c r="L19" s="36"/>
-      <c r="M19" s="50">
+      <c r="J19" s="50" t="s">
+        <v>17</v>
+      </c>
+      <c r="K19" s="50"/>
+      <c r="L19" s="50"/>
+      <c r="M19" s="42">
         <f>ABS((M12-M14)/M12)</f>
         <v>9.8438137256995888E-3</v>
       </c>
-      <c r="N19" s="50"/>
+      <c r="N19" s="42"/>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" s="29" t="s">
@@ -16283,23 +16292,23 @@
         <f>AVERAGE(B4:B18)</f>
         <v>3.9533333333333336</v>
       </c>
-      <c r="C20" s="38"/>
+      <c r="C20" s="34"/>
       <c r="D20" s="19">
         <f>AVERAGE(D4:D18)</f>
         <v>8.4720466666666668E-3</v>
       </c>
-      <c r="E20" s="41"/>
+      <c r="E20" s="37"/>
       <c r="F20" s="19">
         <f>AVERAGE(F4:F18)</f>
         <v>467.27349049454619</v>
       </c>
-      <c r="G20" s="44"/>
-      <c r="H20" s="44"/>
-      <c r="J20" s="36"/>
-      <c r="K20" s="36"/>
-      <c r="L20" s="36"/>
-      <c r="M20" s="50"/>
-      <c r="N20" s="50"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="40"/>
+      <c r="J20" s="50"/>
+      <c r="K20" s="50"/>
+      <c r="L20" s="50"/>
+      <c r="M20" s="42"/>
+      <c r="N20" s="42"/>
     </row>
     <row r="21" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="29" t="s">
@@ -16309,28 +16318,28 @@
         <f>STDEVA(B4:B18)</f>
         <v>2.187825622023142</v>
       </c>
-      <c r="C21" s="39"/>
+      <c r="C21" s="35"/>
       <c r="D21" s="19">
         <f>STDEVA(D4:D18)</f>
         <v>4.7011902788954372E-3</v>
       </c>
-      <c r="E21" s="42"/>
+      <c r="E21" s="38"/>
       <c r="F21" s="19">
         <f>STDEVA(F4:F18)</f>
         <v>1.8649100465002957</v>
       </c>
-      <c r="G21" s="44"/>
-      <c r="H21" s="44"/>
-      <c r="J21" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="K21" s="31"/>
-      <c r="L21" s="31"/>
-      <c r="M21" s="45">
+      <c r="G21" s="40"/>
+      <c r="H21" s="40"/>
+      <c r="J21" s="46" t="s">
+        <v>20</v>
+      </c>
+      <c r="K21" s="49"/>
+      <c r="L21" s="49"/>
+      <c r="M21" s="41">
         <f>ABS((M12-F20)/M12)</f>
         <v>5.8010840541570319E-3</v>
       </c>
-      <c r="N21" s="45"/>
+      <c r="N21" s="41"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" s="29" t="s">
@@ -16340,23 +16349,23 @@
         <f>B21/SQRT(10)</f>
         <v>0.69185120888677698</v>
       </c>
-      <c r="C22" s="40"/>
+      <c r="C22" s="36"/>
       <c r="D22" s="19">
         <f>D21/SQRT(10)</f>
         <v>1.4866468995151792E-3</v>
       </c>
-      <c r="E22" s="43"/>
+      <c r="E22" s="39"/>
       <c r="F22" s="19">
         <f t="shared" ref="F22" si="1">F21/SQRT(10)</f>
         <v>0.58973633782714585</v>
       </c>
-      <c r="G22" s="44"/>
-      <c r="H22" s="44"/>
-      <c r="J22" s="31"/>
-      <c r="K22" s="31"/>
-      <c r="L22" s="31"/>
-      <c r="M22" s="45"/>
-      <c r="N22" s="45"/>
+      <c r="G22" s="40"/>
+      <c r="H22" s="40"/>
+      <c r="J22" s="49"/>
+      <c r="K22" s="49"/>
+      <c r="L22" s="49"/>
+      <c r="M22" s="41"/>
+      <c r="N22" s="41"/>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="I27" s="1"/>
@@ -17612,12 +17621,15 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="M4:N7"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="J10:L10"/>
+    <mergeCell ref="J15:L15"/>
+    <mergeCell ref="J17:L17"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="J16:L16"/>
+    <mergeCell ref="J14:L14"/>
+    <mergeCell ref="J12:L12"/>
+    <mergeCell ref="J11:L11"/>
     <mergeCell ref="C20:C22"/>
     <mergeCell ref="E20:E22"/>
     <mergeCell ref="G20:H22"/>
@@ -17625,17 +17637,14 @@
     <mergeCell ref="M16:N16"/>
     <mergeCell ref="M17:N17"/>
     <mergeCell ref="M19:N20"/>
-    <mergeCell ref="J10:L10"/>
-    <mergeCell ref="J15:L15"/>
-    <mergeCell ref="J17:L17"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="J3:K3"/>
     <mergeCell ref="J21:L22"/>
-    <mergeCell ref="J16:L16"/>
-    <mergeCell ref="J14:L14"/>
-    <mergeCell ref="J12:L12"/>
-    <mergeCell ref="J11:L11"/>
     <mergeCell ref="J19:L20"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="M4:N7"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="M14:N14"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="9.8425196850393706E-2" bottom="9.8425196850393706E-2" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -17669,8 +17678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FFE3FEA-051F-43E6-A195-9D45A472FA48}">
   <dimension ref="A2:Y161"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17692,47 +17701,47 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A2" s="37" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
+      <c r="A2" s="47" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="E3" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="21" t="s">
-        <v>12</v>
-      </c>
       <c r="G3" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="1"/>
-      <c r="J3" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="K3" s="32"/>
+      <c r="K3" s="48"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" s="28">
@@ -17997,15 +18006,15 @@
         <v>0.35170041002550789</v>
       </c>
       <c r="I10" s="1"/>
-      <c r="J10" s="33" t="s">
+      <c r="J10" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="K10" s="34"/>
-      <c r="L10" s="35"/>
-      <c r="M10" s="47">
+      <c r="K10" s="44"/>
+      <c r="L10" s="45"/>
+      <c r="M10" s="30">
         <v>0.01</v>
       </c>
-      <c r="N10" s="47"/>
+      <c r="N10" s="30"/>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11" s="28">
@@ -18036,15 +18045,15 @@
         <v>-2.0605841003705549E-2</v>
       </c>
       <c r="I11" s="1"/>
-      <c r="J11" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="K11" s="34"/>
-      <c r="L11" s="35"/>
-      <c r="M11" s="47">
+      <c r="J11" s="43" t="s">
+        <v>11</v>
+      </c>
+      <c r="K11" s="44"/>
+      <c r="L11" s="45"/>
+      <c r="M11" s="30">
         <v>9.9999999999999995E-8</v>
       </c>
-      <c r="N11" s="47"/>
+      <c r="N11" s="30"/>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12" s="28">
@@ -18075,15 +18084,15 @@
         <v>-1.6446095729433452E-2</v>
       </c>
       <c r="I12" s="1"/>
-      <c r="J12" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="K12" s="34"/>
-      <c r="L12" s="35"/>
-      <c r="M12" s="47">
+      <c r="J12" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="K12" s="44"/>
+      <c r="L12" s="45"/>
+      <c r="M12" s="30">
         <v>10000</v>
       </c>
-      <c r="N12" s="47"/>
+      <c r="N12" s="30"/>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A13" s="28">
@@ -18148,16 +18157,16 @@
         <v>-1.5310768080984971E-2</v>
       </c>
       <c r="I14" s="1"/>
-      <c r="J14" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="K14" s="34"/>
-      <c r="L14" s="35"/>
-      <c r="M14" s="47">
+      <c r="J14" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="K14" s="44"/>
+      <c r="L14" s="45"/>
+      <c r="M14" s="30">
         <f>J4</f>
         <v>10104.290262959434</v>
       </c>
-      <c r="N14" s="47"/>
+      <c r="N14" s="30"/>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A15" s="28">
@@ -18188,16 +18197,16 @@
         <v>-2.2193925436306827E-2</v>
       </c>
       <c r="I15" s="1"/>
-      <c r="J15" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="K15" s="34"/>
-      <c r="L15" s="35"/>
-      <c r="M15" s="48">
+      <c r="J15" s="43" t="s">
+        <v>31</v>
+      </c>
+      <c r="K15" s="44"/>
+      <c r="L15" s="45"/>
+      <c r="M15" s="32">
         <f>J5</f>
         <v>89.573503681548132</v>
       </c>
-      <c r="N15" s="48"/>
+      <c r="N15" s="32"/>
     </row>
     <row r="16" spans="1:24" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="28">
@@ -18228,16 +18237,16 @@
         <v>-1.7721309373159855E-2</v>
       </c>
       <c r="I16" s="1"/>
-      <c r="J16" s="32" t="s">
-        <v>35</v>
-      </c>
-      <c r="K16" s="32"/>
-      <c r="L16" s="32"/>
-      <c r="M16" s="47">
+      <c r="J16" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="K16" s="48"/>
+      <c r="L16" s="48"/>
+      <c r="M16" s="30">
         <f>F20</f>
         <v>10013.978027113197</v>
       </c>
-      <c r="N16" s="47"/>
+      <c r="N16" s="30"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="28">
@@ -18268,11 +18277,11 @@
         <v>-2.1162888050820783E-2</v>
       </c>
       <c r="I17" s="1"/>
-      <c r="J17" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="K17" s="30"/>
-      <c r="L17" s="30"/>
+      <c r="J17" s="46" t="s">
+        <v>21</v>
+      </c>
+      <c r="K17" s="46"/>
+      <c r="L17" s="46"/>
       <c r="M17" s="51">
         <f>SQRT(((1/D20)*B22)^2+(-(B20/(D20^2))*D22)^2)</f>
         <v>2275.6957077765142</v>
@@ -18315,16 +18324,16 @@
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-      <c r="J19" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="K19" s="36"/>
-      <c r="L19" s="36"/>
-      <c r="M19" s="50">
+      <c r="J19" s="50" t="s">
+        <v>17</v>
+      </c>
+      <c r="K19" s="50"/>
+      <c r="L19" s="50"/>
+      <c r="M19" s="42">
         <f>ABS((M12-M14)/M12)</f>
         <v>1.0429026295943368E-2</v>
       </c>
-      <c r="N19" s="50"/>
+      <c r="N19" s="42"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="29" t="s">
@@ -18334,23 +18343,23 @@
         <f>AVERAGE(B4:B18)</f>
         <v>6.1260000000000003</v>
       </c>
-      <c r="C20" s="38"/>
+      <c r="C20" s="34"/>
       <c r="D20" s="19">
         <f>AVERAGE(D4:D18)</f>
         <v>6.0826666666666663E-4</v>
       </c>
-      <c r="E20" s="41"/>
+      <c r="E20" s="37"/>
       <c r="F20" s="19">
         <f>AVERAGE(F4:F18)</f>
         <v>10013.978027113197</v>
       </c>
-      <c r="G20" s="44"/>
-      <c r="H20" s="44"/>
-      <c r="J20" s="36"/>
-      <c r="K20" s="36"/>
-      <c r="L20" s="36"/>
-      <c r="M20" s="50"/>
-      <c r="N20" s="50"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="40"/>
+      <c r="J20" s="50"/>
+      <c r="K20" s="50"/>
+      <c r="L20" s="50"/>
+      <c r="M20" s="42"/>
+      <c r="N20" s="42"/>
     </row>
     <row r="21" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="29" t="s">
@@ -18360,28 +18369,28 @@
         <f>STDEVA(B4:B18)</f>
         <v>3.1010869062314277</v>
       </c>
-      <c r="C21" s="39"/>
+      <c r="C21" s="35"/>
       <c r="D21" s="19">
         <f>STDEVA(D4:D18)</f>
         <v>3.0675128749681294E-4</v>
       </c>
-      <c r="E21" s="42"/>
+      <c r="E21" s="38"/>
       <c r="F21" s="19">
         <f>STDEVA(F4:F18)</f>
         <v>261.13897472485797</v>
       </c>
-      <c r="G21" s="44"/>
-      <c r="H21" s="44"/>
-      <c r="J21" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="K21" s="31"/>
-      <c r="L21" s="31"/>
-      <c r="M21" s="45">
+      <c r="G21" s="40"/>
+      <c r="H21" s="40"/>
+      <c r="J21" s="46" t="s">
+        <v>20</v>
+      </c>
+      <c r="K21" s="49"/>
+      <c r="L21" s="49"/>
+      <c r="M21" s="41">
         <f>ABS((M12-F20)/M12)</f>
         <v>1.3978027113196732E-3</v>
       </c>
-      <c r="N21" s="45"/>
+      <c r="N21" s="41"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="29" t="s">
@@ -18391,23 +18400,23 @@
         <f>B21/SQRT(10)</f>
         <v>0.98064978458163166</v>
       </c>
-      <c r="C22" s="40"/>
+      <c r="C22" s="36"/>
       <c r="D22" s="19">
         <f>D21/SQRT(10)</f>
         <v>9.7003274367905937E-5</v>
       </c>
-      <c r="E22" s="43"/>
+      <c r="E22" s="39"/>
       <c r="F22" s="19">
         <f t="shared" ref="F22" si="1">F21/SQRT(10)</f>
         <v>82.57939459716934</v>
       </c>
-      <c r="G22" s="44"/>
-      <c r="H22" s="44"/>
-      <c r="J22" s="31"/>
-      <c r="K22" s="31"/>
-      <c r="L22" s="31"/>
-      <c r="M22" s="45"/>
-      <c r="N22" s="45"/>
+      <c r="G22" s="40"/>
+      <c r="H22" s="40"/>
+      <c r="J22" s="49"/>
+      <c r="K22" s="49"/>
+      <c r="L22" s="49"/>
+      <c r="M22" s="41"/>
+      <c r="N22" s="41"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="I27" s="1"/>
@@ -19662,6 +19671,22 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="J21:L22"/>
+    <mergeCell ref="J19:L20"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="E20:E22"/>
+    <mergeCell ref="G20:H22"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="J12:L12"/>
+    <mergeCell ref="J14:L14"/>
+    <mergeCell ref="J10:L10"/>
+    <mergeCell ref="J15:L15"/>
+    <mergeCell ref="J17:L17"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="J16:L16"/>
     <mergeCell ref="M21:N22"/>
     <mergeCell ref="M16:N16"/>
     <mergeCell ref="M10:N10"/>
@@ -19669,22 +19694,6 @@
     <mergeCell ref="M12:N12"/>
     <mergeCell ref="M14:N14"/>
     <mergeCell ref="M19:N20"/>
-    <mergeCell ref="J15:L15"/>
-    <mergeCell ref="J17:L17"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="J16:L16"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="J12:L12"/>
-    <mergeCell ref="J14:L14"/>
-    <mergeCell ref="J10:L10"/>
-    <mergeCell ref="J21:L22"/>
-    <mergeCell ref="J19:L20"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="E20:E22"/>
-    <mergeCell ref="G20:H22"/>
   </mergeCells>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="9.8425196850393706E-2" bottom="9.8425196850393706E-2" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -19700,7 +19709,7 @@
   <dimension ref="A2:Y161"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20:C22"/>
+      <selection activeCell="A2" sqref="A2:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19722,47 +19731,47 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A2" s="37" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
+      <c r="A2" s="47" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="E3" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="21" t="s">
-        <v>12</v>
-      </c>
       <c r="G3" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="1"/>
-      <c r="J3" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="K3" s="32"/>
+      <c r="K3" s="48"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" s="28">
@@ -20027,15 +20036,15 @@
         <v>-7.6810709253170906E-2</v>
       </c>
       <c r="I10" s="1"/>
-      <c r="J10" s="33" t="s">
+      <c r="J10" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="K10" s="34"/>
-      <c r="L10" s="35"/>
-      <c r="M10" s="47">
+      <c r="K10" s="44"/>
+      <c r="L10" s="45"/>
+      <c r="M10" s="30">
         <v>0.01</v>
       </c>
-      <c r="N10" s="47"/>
+      <c r="N10" s="30"/>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11" s="28">
@@ -20066,15 +20075,15 @@
         <v>1.5669328323156151E-2</v>
       </c>
       <c r="I11" s="1"/>
-      <c r="J11" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="K11" s="34"/>
-      <c r="L11" s="35"/>
-      <c r="M11" s="47">
+      <c r="J11" s="43" t="s">
+        <v>11</v>
+      </c>
+      <c r="K11" s="44"/>
+      <c r="L11" s="45"/>
+      <c r="M11" s="30">
         <v>9.9999999999999995E-8</v>
       </c>
-      <c r="N11" s="47"/>
+      <c r="N11" s="30"/>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12" s="28">
@@ -20105,15 +20114,15 @@
         <v>7.8149365899482959E-2</v>
       </c>
       <c r="I12" s="1"/>
-      <c r="J12" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="K12" s="34"/>
-      <c r="L12" s="35"/>
-      <c r="M12" s="47">
+      <c r="J12" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="K12" s="44"/>
+      <c r="L12" s="45"/>
+      <c r="M12" s="30">
         <v>6800000</v>
       </c>
-      <c r="N12" s="47"/>
+      <c r="N12" s="30"/>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A13" s="28">
@@ -20178,16 +20187,16 @@
         <v>-6.1930483795210378E-2</v>
       </c>
       <c r="I14" s="1"/>
-      <c r="J14" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="K14" s="34"/>
-      <c r="L14" s="35"/>
-      <c r="M14" s="47">
+      <c r="J14" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="K14" s="44"/>
+      <c r="L14" s="45"/>
+      <c r="M14" s="30">
         <f>J4</f>
         <v>4175199.6242367309</v>
       </c>
-      <c r="N14" s="47"/>
+      <c r="N14" s="30"/>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A15" s="28">
@@ -20218,11 +20227,11 @@
         <v>-0.18697040864255676</v>
       </c>
       <c r="I15" s="1"/>
-      <c r="J15" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="K15" s="34"/>
-      <c r="L15" s="35"/>
+      <c r="J15" s="43" t="s">
+        <v>31</v>
+      </c>
+      <c r="K15" s="44"/>
+      <c r="L15" s="45"/>
       <c r="M15" s="51">
         <f>J5</f>
         <v>58948.507012604212</v>
@@ -20259,15 +20268,15 @@
       </c>
       <c r="I16" s="1"/>
       <c r="J16" s="52" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="K16" s="52"/>
       <c r="L16" s="52"/>
-      <c r="M16" s="47">
+      <c r="M16" s="30">
         <f>F20</f>
         <v>3394887.6612494262</v>
       </c>
-      <c r="N16" s="47"/>
+      <c r="N16" s="30"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="28">
@@ -20298,11 +20307,11 @@
         <v>7.5509628933771111E-2</v>
       </c>
       <c r="I17" s="1"/>
-      <c r="J17" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="K17" s="30"/>
-      <c r="L17" s="30"/>
+      <c r="J17" s="46" t="s">
+        <v>21</v>
+      </c>
+      <c r="K17" s="46"/>
+      <c r="L17" s="46"/>
       <c r="M17" s="51">
         <f>SQRT(((1/D20)*B22)^2+(-(B20/(D20^2))*D22)^2)</f>
         <v>641862.27200783929</v>
@@ -20345,16 +20354,16 @@
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-      <c r="J19" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="K19" s="36"/>
-      <c r="L19" s="36"/>
-      <c r="M19" s="50">
+      <c r="J19" s="50" t="s">
+        <v>17</v>
+      </c>
+      <c r="K19" s="50"/>
+      <c r="L19" s="50"/>
+      <c r="M19" s="42">
         <f>ABS((M12-M14)/M12)</f>
         <v>0.38600005525930431</v>
       </c>
-      <c r="N19" s="50"/>
+      <c r="N19" s="42"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="29" t="s">
@@ -20364,23 +20373,23 @@
         <f>AVERAGE(B4:B18)</f>
         <v>6.02</v>
       </c>
-      <c r="C20" s="38"/>
+      <c r="C20" s="34"/>
       <c r="D20" s="19">
         <f>AVERAGE(D4:D18)</f>
         <v>1.7133333333333332E-6</v>
       </c>
-      <c r="E20" s="41"/>
+      <c r="E20" s="37"/>
       <c r="F20" s="19">
         <f>AVERAGE(F4:F18)</f>
         <v>3394887.6612494262</v>
       </c>
-      <c r="G20" s="44"/>
-      <c r="H20" s="44"/>
-      <c r="J20" s="36"/>
-      <c r="K20" s="36"/>
-      <c r="L20" s="36"/>
-      <c r="M20" s="50"/>
-      <c r="N20" s="50"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="40"/>
+      <c r="J20" s="50"/>
+      <c r="K20" s="50"/>
+      <c r="L20" s="50"/>
+      <c r="M20" s="42"/>
+      <c r="N20" s="42"/>
     </row>
     <row r="21" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="29" t="s">
@@ -20390,28 +20399,28 @@
         <f>STDEVA(B4:B18)</f>
         <v>2.66224126844818</v>
       </c>
-      <c r="C21" s="39"/>
+      <c r="C21" s="35"/>
       <c r="D21" s="19">
         <f>STDEVA(D4:D18)</f>
         <v>6.3680751371494486E-7</v>
       </c>
-      <c r="E21" s="42"/>
+      <c r="E21" s="38"/>
       <c r="F21" s="19">
         <f>STDEVA(F4:F18)</f>
         <v>394535.0166596687</v>
       </c>
-      <c r="G21" s="44"/>
-      <c r="H21" s="44"/>
-      <c r="J21" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="K21" s="31"/>
-      <c r="L21" s="31"/>
-      <c r="M21" s="45">
+      <c r="G21" s="40"/>
+      <c r="H21" s="40"/>
+      <c r="J21" s="46" t="s">
+        <v>20</v>
+      </c>
+      <c r="K21" s="49"/>
+      <c r="L21" s="49"/>
+      <c r="M21" s="41">
         <f>ABS((M12-F20)/M12)</f>
         <v>0.50075181452214323</v>
       </c>
-      <c r="N21" s="45"/>
+      <c r="N21" s="41"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="29" t="s">
@@ -20421,23 +20430,23 @@
         <f>B21/SQRT(10)</f>
         <v>0.84187460891920085</v>
       </c>
-      <c r="C22" s="40"/>
+      <c r="C22" s="36"/>
       <c r="D22" s="19">
         <f>D21/SQRT(10)</f>
         <v>2.0137621744481388E-7</v>
       </c>
-      <c r="E22" s="43"/>
+      <c r="E22" s="39"/>
       <c r="F22" s="19">
         <f t="shared" ref="F22" si="1">F21/SQRT(10)</f>
         <v>124762.92693370297</v>
       </c>
-      <c r="G22" s="44"/>
-      <c r="H22" s="44"/>
-      <c r="J22" s="31"/>
-      <c r="K22" s="31"/>
-      <c r="L22" s="31"/>
-      <c r="M22" s="45"/>
-      <c r="N22" s="45"/>
+      <c r="G22" s="40"/>
+      <c r="H22" s="40"/>
+      <c r="J22" s="49"/>
+      <c r="K22" s="49"/>
+      <c r="L22" s="49"/>
+      <c r="M22" s="41"/>
+      <c r="N22" s="41"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="I27" s="1"/>
@@ -21692,6 +21701,22 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="J21:L22"/>
+    <mergeCell ref="J19:L20"/>
+    <mergeCell ref="G20:H22"/>
+    <mergeCell ref="E20:E22"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="J12:L12"/>
+    <mergeCell ref="J14:L14"/>
+    <mergeCell ref="J10:L10"/>
+    <mergeCell ref="J15:L15"/>
+    <mergeCell ref="J17:L17"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="J16:L16"/>
     <mergeCell ref="M21:N22"/>
     <mergeCell ref="M16:N16"/>
     <mergeCell ref="M10:N10"/>
@@ -21699,22 +21724,6 @@
     <mergeCell ref="M12:N12"/>
     <mergeCell ref="M14:N14"/>
     <mergeCell ref="M19:N20"/>
-    <mergeCell ref="J15:L15"/>
-    <mergeCell ref="J17:L17"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="J16:L16"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="J12:L12"/>
-    <mergeCell ref="J14:L14"/>
-    <mergeCell ref="J10:L10"/>
-    <mergeCell ref="J21:L22"/>
-    <mergeCell ref="J19:L20"/>
-    <mergeCell ref="G20:H22"/>
-    <mergeCell ref="E20:E22"/>
-    <mergeCell ref="C20:C22"/>
   </mergeCells>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="9.8425196850393706E-2" bottom="9.8425196850393706E-2" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -21729,8 +21738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD8B41A8-119D-45F7-AE39-7CD01A0BBCB0}">
   <dimension ref="A2:Y161"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R17" sqref="R17"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -21752,47 +21761,47 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A2" s="37" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
+      <c r="A2" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="E3" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="23" t="s">
-        <v>12</v>
-      </c>
       <c r="G3" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="1"/>
-      <c r="J3" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="K3" s="32"/>
+      <c r="K3" s="48"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" s="28">
@@ -21808,7 +21817,7 @@
         <v>1.714E-3</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F4" s="5">
         <f t="shared" ref="F4:F18" si="0">B4/D4</f>
@@ -21830,10 +21839,10 @@
       <c r="K4" s="22">
         <v>8.0902685690213971E-3</v>
       </c>
-      <c r="M4" s="49" t="s">
-        <v>33</v>
-      </c>
-      <c r="N4" s="49"/>
+      <c r="M4" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="N4" s="33"/>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="28">
@@ -21849,7 +21858,7 @@
         <v>3.0699999999999998E-3</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F5" s="5">
         <f t="shared" si="0"/>
@@ -21870,8 +21879,8 @@
       <c r="K5" s="22">
         <v>1.2743622496404835E-2</v>
       </c>
-      <c r="M5" s="49"/>
-      <c r="N5" s="49"/>
+      <c r="M5" s="33"/>
+      <c r="N5" s="33"/>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" s="28">
@@ -21887,7 +21896,7 @@
         <v>4.7404999999999999E-3</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F6" s="5">
         <f t="shared" si="0"/>
@@ -21908,8 +21917,8 @@
       <c r="K6" s="22">
         <v>2.2511589962947894E-2</v>
       </c>
-      <c r="M6" s="49"/>
-      <c r="N6" s="49"/>
+      <c r="M6" s="33"/>
+      <c r="N6" s="33"/>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" s="28">
@@ -21925,7 +21934,7 @@
         <v>6.5395000000000002E-3</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F7" s="5">
         <f t="shared" si="0"/>
@@ -21947,8 +21956,8 @@
         <v>13</v>
       </c>
       <c r="L7" s="1"/>
-      <c r="M7" s="49"/>
-      <c r="N7" s="49"/>
+      <c r="M7" s="33"/>
+      <c r="N7" s="33"/>
       <c r="O7" s="3"/>
       <c r="P7" s="23"/>
       <c r="Q7" s="3"/>
@@ -21970,7 +21979,7 @@
         <v>7.8584999999999992E-3</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F8" s="5">
         <f t="shared" si="0"/>
@@ -22009,7 +22018,7 @@
         <v>9.6395000000000005E-3</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F9" s="5">
         <f t="shared" si="0"/>
@@ -22044,7 +22053,7 @@
         <v>1.0932000000000001E-2</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F10" s="5">
         <f t="shared" si="0"/>
@@ -22059,15 +22068,15 @@
         <v>2.2408934246589851E-2</v>
       </c>
       <c r="I10" s="1"/>
-      <c r="J10" s="33" t="s">
+      <c r="J10" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="K10" s="34"/>
-      <c r="L10" s="35"/>
-      <c r="M10" s="47">
+      <c r="K10" s="44"/>
+      <c r="L10" s="45"/>
+      <c r="M10" s="30">
         <v>0.01</v>
       </c>
-      <c r="N10" s="47"/>
+      <c r="N10" s="30"/>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11" s="28">
@@ -22083,7 +22092,7 @@
         <v>1.2722499999999999E-2</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F11" s="5">
         <f t="shared" si="0"/>
@@ -22098,15 +22107,15 @@
         <v>-1.176061852810939E-3</v>
       </c>
       <c r="I11" s="1"/>
-      <c r="J11" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="K11" s="34"/>
-      <c r="L11" s="35"/>
-      <c r="M11" s="47">
+      <c r="J11" s="43" t="s">
+        <v>11</v>
+      </c>
+      <c r="K11" s="44"/>
+      <c r="L11" s="45"/>
+      <c r="M11" s="30">
         <v>9.9999999999999995E-8</v>
       </c>
-      <c r="N11" s="47"/>
+      <c r="N11" s="30"/>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12" s="28">
@@ -22122,7 +22131,7 @@
         <v>1.465E-2</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F12" s="5">
         <f t="shared" si="0"/>
@@ -22137,15 +22146,15 @@
         <v>1.4572361189317817E-3</v>
       </c>
       <c r="I12" s="1"/>
-      <c r="J12" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="K12" s="34"/>
-      <c r="L12" s="35"/>
-      <c r="M12" s="46">
+      <c r="J12" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="K12" s="44"/>
+      <c r="L12" s="45"/>
+      <c r="M12" s="31">
         <v>470</v>
       </c>
-      <c r="N12" s="46"/>
+      <c r="N12" s="31"/>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A13" s="28">
@@ -22197,7 +22206,7 @@
         <v>1.7070999999999999E-2</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F14" s="5">
         <f t="shared" si="0"/>
@@ -22212,16 +22221,16 @@
         <v>4.3367247776027185E-3</v>
       </c>
       <c r="I14" s="1"/>
-      <c r="J14" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="K14" s="34"/>
-      <c r="L14" s="35"/>
-      <c r="M14" s="46">
+      <c r="J14" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="K14" s="44"/>
+      <c r="L14" s="45"/>
+      <c r="M14" s="31">
         <f>J4</f>
         <v>465.55989729092471</v>
       </c>
-      <c r="N14" s="46"/>
+      <c r="N14" s="31"/>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A15" s="28">
@@ -22237,7 +22246,7 @@
         <v>1.8512500000000001E-2</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F15" s="5">
         <f t="shared" si="0"/>
@@ -22252,16 +22261,16 @@
         <v>3.232132832733825E-3</v>
       </c>
       <c r="I15" s="1"/>
-      <c r="J15" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="K15" s="34"/>
-      <c r="L15" s="35"/>
-      <c r="M15" s="48">
+      <c r="J15" s="43" t="s">
+        <v>31</v>
+      </c>
+      <c r="K15" s="44"/>
+      <c r="L15" s="45"/>
+      <c r="M15" s="32">
         <f>J5</f>
         <v>0.92403458921281356</v>
       </c>
-      <c r="N15" s="48"/>
+      <c r="N15" s="32"/>
     </row>
     <row r="16" spans="1:24" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="28">
@@ -22277,7 +22286,7 @@
         <v>1.9453999999999999E-2</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F16" s="5">
         <f t="shared" si="0"/>
@@ -22292,16 +22301,16 @@
         <v>-5.0925104666692533E-3</v>
       </c>
       <c r="I16" s="1"/>
-      <c r="J16" s="32" t="s">
-        <v>35</v>
-      </c>
-      <c r="K16" s="32"/>
-      <c r="L16" s="32"/>
-      <c r="M16" s="46">
+      <c r="J16" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="K16" s="48"/>
+      <c r="L16" s="48"/>
+      <c r="M16" s="31">
         <f>F20</f>
         <v>466.47899063055797</v>
       </c>
-      <c r="N16" s="46"/>
+      <c r="N16" s="31"/>
     </row>
     <row r="17" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="28">
@@ -22332,16 +22341,16 @@
         <v>-7.1320951526505638E-3</v>
       </c>
       <c r="I17" s="1"/>
-      <c r="J17" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="K17" s="30"/>
-      <c r="L17" s="30"/>
-      <c r="M17" s="48">
+      <c r="J17" s="46" t="s">
+        <v>21</v>
+      </c>
+      <c r="K17" s="46"/>
+      <c r="L17" s="46"/>
+      <c r="M17" s="32">
         <f>SQRT(((1/D20)*B22)^2+(-(B20/(D20^2))*D22)^2)</f>
         <v>110.53496611955116</v>
       </c>
-      <c r="N17" s="48"/>
+      <c r="N17" s="32"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="28">
@@ -22379,16 +22388,16 @@
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-      <c r="J19" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="K19" s="36"/>
-      <c r="L19" s="36"/>
-      <c r="M19" s="50">
+      <c r="J19" s="50" t="s">
+        <v>17</v>
+      </c>
+      <c r="K19" s="50"/>
+      <c r="L19" s="50"/>
+      <c r="M19" s="42">
         <f>ABS((M12-M14)/M12)</f>
         <v>9.4470270405857242E-3</v>
       </c>
-      <c r="N19" s="50"/>
+      <c r="N19" s="42"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="29" t="s">
@@ -22398,23 +22407,23 @@
         <f>AVERAGE(B4:B18)</f>
         <v>5.7219999999999995</v>
       </c>
-      <c r="C20" s="38"/>
+      <c r="C20" s="34"/>
       <c r="D20" s="19">
         <f>AVERAGE(D4:D18)</f>
         <v>1.2273200000000001E-2</v>
       </c>
-      <c r="E20" s="41"/>
+      <c r="E20" s="37"/>
       <c r="F20" s="19">
         <f>AVERAGE(F4:F18)</f>
         <v>466.47899063055797</v>
       </c>
-      <c r="G20" s="44"/>
-      <c r="H20" s="44"/>
-      <c r="J20" s="36"/>
-      <c r="K20" s="36"/>
-      <c r="L20" s="36"/>
-      <c r="M20" s="50"/>
-      <c r="N20" s="50"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="40"/>
+      <c r="J20" s="50"/>
+      <c r="K20" s="50"/>
+      <c r="L20" s="50"/>
+      <c r="M20" s="42"/>
+      <c r="N20" s="42"/>
     </row>
     <row r="21" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="29" t="s">
@@ -22424,28 +22433,28 @@
         <f>STDEVA(B4:B18)</f>
         <v>3.031381580354787</v>
       </c>
-      <c r="C21" s="39"/>
+      <c r="C21" s="35"/>
       <c r="D21" s="19">
         <f>STDEVA(D4:D18)</f>
         <v>6.5110933737298335E-3</v>
       </c>
-      <c r="E21" s="42"/>
+      <c r="E21" s="38"/>
       <c r="F21" s="19">
         <f>STDEVA(F4:F18)</f>
         <v>4.1032210501884805</v>
       </c>
-      <c r="G21" s="44"/>
-      <c r="H21" s="44"/>
-      <c r="J21" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="K21" s="31"/>
-      <c r="L21" s="31"/>
-      <c r="M21" s="45">
+      <c r="G21" s="40"/>
+      <c r="H21" s="40"/>
+      <c r="J21" s="46" t="s">
+        <v>20</v>
+      </c>
+      <c r="K21" s="49"/>
+      <c r="L21" s="49"/>
+      <c r="M21" s="41">
         <f>ABS((M12-F20)/M12)</f>
         <v>7.4915092966851629E-3</v>
       </c>
-      <c r="N21" s="45"/>
+      <c r="N21" s="41"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="29" t="s">
@@ -22455,23 +22464,23 @@
         <f>B21/SQRT(10)</f>
         <v>0.95860702510018592</v>
       </c>
-      <c r="C22" s="40"/>
+      <c r="C22" s="36"/>
       <c r="D22" s="19">
         <f>D21/SQRT(10)</f>
         <v>2.0589885119016217E-3</v>
       </c>
-      <c r="E22" s="43"/>
+      <c r="E22" s="39"/>
       <c r="F22" s="19">
         <f t="shared" ref="F22" si="1">F21/SQRT(10)</f>
         <v>1.2975524261743667</v>
       </c>
-      <c r="G22" s="44"/>
-      <c r="H22" s="44"/>
-      <c r="J22" s="31"/>
-      <c r="K22" s="31"/>
-      <c r="L22" s="31"/>
-      <c r="M22" s="45"/>
-      <c r="N22" s="45"/>
+      <c r="G22" s="40"/>
+      <c r="H22" s="40"/>
+      <c r="J22" s="49"/>
+      <c r="K22" s="49"/>
+      <c r="L22" s="49"/>
+      <c r="M22" s="41"/>
+      <c r="N22" s="41"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="I27" s="1"/>
@@ -23726,6 +23735,16 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="J19:L20"/>
+    <mergeCell ref="J21:L22"/>
+    <mergeCell ref="J10:L10"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="J12:L12"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="E20:E22"/>
+    <mergeCell ref="G20:H22"/>
     <mergeCell ref="M19:N20"/>
     <mergeCell ref="M21:N22"/>
     <mergeCell ref="M4:N7"/>
@@ -23740,16 +23759,6 @@
     <mergeCell ref="M14:N14"/>
     <mergeCell ref="M15:N15"/>
     <mergeCell ref="M17:N17"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="J19:L20"/>
-    <mergeCell ref="J21:L22"/>
-    <mergeCell ref="J10:L10"/>
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="J12:L12"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="E20:E22"/>
-    <mergeCell ref="G20:H22"/>
   </mergeCells>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="9.8425196850393706E-2" bottom="9.8425196850393706E-2" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -23765,7 +23774,7 @@
   <dimension ref="A2:Y161"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4:N7"/>
+      <selection activeCell="A2" sqref="A2:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23787,47 +23796,47 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A2" s="37" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
+      <c r="A2" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="E3" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="23" t="s">
-        <v>12</v>
-      </c>
       <c r="G3" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="1"/>
-      <c r="J3" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="K3" s="32"/>
+      <c r="K3" s="48"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" s="28">
@@ -23865,10 +23874,10 @@
       <c r="K4" s="22">
         <v>1.0421637951800733E-3</v>
       </c>
-      <c r="M4" s="49" t="s">
-        <v>33</v>
-      </c>
-      <c r="N4" s="49"/>
+      <c r="M4" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="N4" s="33"/>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="28">
@@ -23878,7 +23887,7 @@
         <v>1.48</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D5" s="7">
         <v>1.46E-4</v>
@@ -23905,8 +23914,8 @@
       <c r="K5" s="22">
         <v>1.058610182411359E-2</v>
       </c>
-      <c r="M5" s="49"/>
-      <c r="N5" s="49"/>
+      <c r="M5" s="33"/>
+      <c r="N5" s="33"/>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" s="28">
@@ -23943,8 +23952,8 @@
       <c r="K6" s="22">
         <v>2.0058815625968805E-2</v>
       </c>
-      <c r="M6" s="49"/>
-      <c r="N6" s="49"/>
+      <c r="M6" s="33"/>
+      <c r="N6" s="33"/>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" s="28">
@@ -23982,8 +23991,8 @@
         <v>13</v>
       </c>
       <c r="L7" s="1"/>
-      <c r="M7" s="49"/>
-      <c r="N7" s="49"/>
+      <c r="M7" s="33"/>
+      <c r="N7" s="33"/>
       <c r="O7" s="3"/>
       <c r="P7" s="23"/>
       <c r="Q7" s="3"/>
@@ -24094,15 +24103,15 @@
         <v>-2.0889005645678971E-3</v>
       </c>
       <c r="I10" s="1"/>
-      <c r="J10" s="33" t="s">
+      <c r="J10" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="K10" s="34"/>
-      <c r="L10" s="35"/>
-      <c r="M10" s="47">
+      <c r="K10" s="44"/>
+      <c r="L10" s="45"/>
+      <c r="M10" s="30">
         <v>0.01</v>
       </c>
-      <c r="N10" s="47"/>
+      <c r="N10" s="30"/>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11" s="28">
@@ -24133,15 +24142,15 @@
         <v>1.4288300483324079E-2</v>
       </c>
       <c r="I11" s="1"/>
-      <c r="J11" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="K11" s="34"/>
-      <c r="L11" s="35"/>
-      <c r="M11" s="47">
+      <c r="J11" s="43" t="s">
+        <v>11</v>
+      </c>
+      <c r="K11" s="44"/>
+      <c r="L11" s="45"/>
+      <c r="M11" s="30">
         <v>9.9999999999999995E-8</v>
       </c>
-      <c r="N11" s="47"/>
+      <c r="N11" s="30"/>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12" s="28">
@@ -24172,15 +24181,15 @@
         <v>1.1585577455561769E-2</v>
       </c>
       <c r="I12" s="1"/>
-      <c r="J12" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="K12" s="34"/>
-      <c r="L12" s="35"/>
-      <c r="M12" s="47">
+      <c r="J12" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="K12" s="44"/>
+      <c r="L12" s="45"/>
+      <c r="M12" s="30">
         <v>10000</v>
       </c>
-      <c r="N12" s="47"/>
+      <c r="N12" s="30"/>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A13" s="28">
@@ -24245,16 +24254,16 @@
         <v>1.4972531749333662E-2</v>
       </c>
       <c r="I14" s="1"/>
-      <c r="J14" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="K14" s="34"/>
-      <c r="L14" s="35"/>
-      <c r="M14" s="47">
+      <c r="J14" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="K14" s="44"/>
+      <c r="L14" s="45"/>
+      <c r="M14" s="30">
         <f>J4</f>
         <v>10057.504745271552</v>
       </c>
-      <c r="N14" s="47"/>
+      <c r="N14" s="30"/>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A15" s="28">
@@ -24285,16 +24294,16 @@
         <v>1.0142133146522347E-2</v>
       </c>
       <c r="I15" s="1"/>
-      <c r="J15" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="K15" s="34"/>
-      <c r="L15" s="35"/>
-      <c r="M15" s="48">
+      <c r="J15" s="43" t="s">
+        <v>31</v>
+      </c>
+      <c r="K15" s="44"/>
+      <c r="L15" s="45"/>
+      <c r="M15" s="32">
         <f>J5</f>
         <v>20.193896080591035</v>
       </c>
-      <c r="N15" s="48"/>
+      <c r="N15" s="32"/>
     </row>
     <row r="16" spans="1:24" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="28">
@@ -24325,16 +24334,16 @@
         <v>1.5369239288983927E-2</v>
       </c>
       <c r="I16" s="1"/>
-      <c r="J16" s="32" t="s">
-        <v>35</v>
-      </c>
-      <c r="K16" s="32"/>
-      <c r="L16" s="32"/>
-      <c r="M16" s="47">
+      <c r="J16" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="K16" s="48"/>
+      <c r="L16" s="48"/>
+      <c r="M16" s="30">
         <f>F20</f>
         <v>10052.067968264466</v>
       </c>
-      <c r="N16" s="47"/>
+      <c r="N16" s="30"/>
     </row>
     <row r="17" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="28">
@@ -24365,11 +24374,11 @@
         <v>-5.9633673549640775E-2</v>
       </c>
       <c r="I17" s="1"/>
-      <c r="J17" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="K17" s="30"/>
-      <c r="L17" s="30"/>
+      <c r="J17" s="46" t="s">
+        <v>21</v>
+      </c>
+      <c r="K17" s="46"/>
+      <c r="L17" s="46"/>
       <c r="M17" s="51">
         <f>SQRT(((1/D20)*B22)^2+(-(B20/(D20^2))*D22)^2)</f>
         <v>2612.0114556618387</v>
@@ -24412,16 +24421,16 @@
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-      <c r="J19" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="K19" s="36"/>
-      <c r="L19" s="36"/>
-      <c r="M19" s="50">
+      <c r="J19" s="50" t="s">
+        <v>17</v>
+      </c>
+      <c r="K19" s="50"/>
+      <c r="L19" s="50"/>
+      <c r="M19" s="42">
         <f>ABS((M12-M14)/M12)</f>
         <v>5.7504745271551652E-3</v>
       </c>
-      <c r="N19" s="50"/>
+      <c r="N19" s="42"/>
     </row>
     <row r="20" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="29" t="s">
@@ -24431,23 +24440,23 @@
         <f>AVERAGE(B4:B18)</f>
         <v>4.5993333333333331</v>
       </c>
-      <c r="C20" s="38"/>
+      <c r="C20" s="34"/>
       <c r="D20" s="19">
         <f>AVERAGE(D4:D18)</f>
         <v>4.5719999999999995E-4</v>
       </c>
-      <c r="E20" s="41"/>
+      <c r="E20" s="37"/>
       <c r="F20" s="19">
         <f>AVERAGE(F4:F18)</f>
         <v>10052.067968264466</v>
       </c>
-      <c r="G20" s="44"/>
-      <c r="H20" s="44"/>
-      <c r="J20" s="36"/>
-      <c r="K20" s="36"/>
-      <c r="L20" s="36"/>
-      <c r="M20" s="50"/>
-      <c r="N20" s="50"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="40"/>
+      <c r="J20" s="50"/>
+      <c r="K20" s="50"/>
+      <c r="L20" s="50"/>
+      <c r="M20" s="42"/>
+      <c r="N20" s="42"/>
     </row>
     <row r="21" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="29" t="s">
@@ -24457,28 +24466,28 @@
         <f>STDEVA(B4:B18)</f>
         <v>2.6700708034129166</v>
       </c>
-      <c r="C21" s="39"/>
+      <c r="C21" s="35"/>
       <c r="D21" s="19">
         <f>STDEVA(D4:D18)</f>
         <v>2.6547348535884221E-4</v>
       </c>
-      <c r="E21" s="42"/>
+      <c r="E21" s="38"/>
       <c r="F21" s="19">
         <f>STDEVA(F4:F18)</f>
         <v>60.017411251811424</v>
       </c>
-      <c r="G21" s="44"/>
-      <c r="H21" s="44"/>
-      <c r="J21" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="K21" s="31"/>
-      <c r="L21" s="31"/>
-      <c r="M21" s="45">
+      <c r="G21" s="40"/>
+      <c r="H21" s="40"/>
+      <c r="J21" s="46" t="s">
+        <v>20</v>
+      </c>
+      <c r="K21" s="49"/>
+      <c r="L21" s="49"/>
+      <c r="M21" s="41">
         <f>ABS((M12-F20)/M12)</f>
         <v>5.2067968264465888E-3</v>
       </c>
-      <c r="N21" s="45"/>
+      <c r="N21" s="41"/>
     </row>
     <row r="22" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="29" t="s">
@@ -24488,23 +24497,23 @@
         <f>B21/SQRT(10)</f>
         <v>0.84435052527005017</v>
       </c>
-      <c r="C22" s="40"/>
+      <c r="C22" s="36"/>
       <c r="D22" s="19">
         <f>D21/SQRT(10)</f>
         <v>8.3950087211730399E-5</v>
       </c>
-      <c r="E22" s="43"/>
+      <c r="E22" s="39"/>
       <c r="F22" s="19">
         <f t="shared" ref="F22" si="1">F21/SQRT(10)</f>
         <v>18.979171882274159</v>
       </c>
-      <c r="G22" s="44"/>
-      <c r="H22" s="44"/>
-      <c r="J22" s="31"/>
-      <c r="K22" s="31"/>
-      <c r="L22" s="31"/>
-      <c r="M22" s="45"/>
-      <c r="N22" s="45"/>
+      <c r="G22" s="40"/>
+      <c r="H22" s="40"/>
+      <c r="J22" s="49"/>
+      <c r="K22" s="49"/>
+      <c r="L22" s="49"/>
+      <c r="M22" s="41"/>
+      <c r="N22" s="41"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="I27" s="1"/>
@@ -25759,19 +25768,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="M4:N7"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="M19:N20"/>
-    <mergeCell ref="M21:N22"/>
-    <mergeCell ref="M16:N16"/>
-    <mergeCell ref="J15:L15"/>
-    <mergeCell ref="J16:L16"/>
-    <mergeCell ref="J17:L17"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="M17:N17"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="J19:L20"/>
@@ -25783,6 +25779,19 @@
     <mergeCell ref="C20:C22"/>
     <mergeCell ref="J10:L10"/>
     <mergeCell ref="J14:L14"/>
+    <mergeCell ref="M19:N20"/>
+    <mergeCell ref="M21:N22"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="J15:L15"/>
+    <mergeCell ref="J16:L16"/>
+    <mergeCell ref="J17:L17"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="M4:N7"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="M14:N14"/>
   </mergeCells>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="9.8425196850393706E-2" bottom="9.8425196850393706E-2" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -25798,7 +25807,7 @@
   <dimension ref="A2:Y161"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17"/>
+      <selection activeCell="A2" sqref="A2:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -25820,47 +25829,47 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A2" s="37" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
+      <c r="A2" s="47" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="E3" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="23" t="s">
-        <v>12</v>
-      </c>
       <c r="G3" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="1"/>
-      <c r="J3" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="K3" s="32"/>
+      <c r="K3" s="48"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" s="28">
@@ -26125,15 +26134,15 @@
         <v>-0.10889512733106077</v>
       </c>
       <c r="I10" s="1"/>
-      <c r="J10" s="33" t="s">
+      <c r="J10" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="K10" s="34"/>
-      <c r="L10" s="35"/>
-      <c r="M10" s="47">
+      <c r="K10" s="44"/>
+      <c r="L10" s="45"/>
+      <c r="M10" s="30">
         <v>0.01</v>
       </c>
-      <c r="N10" s="47"/>
+      <c r="N10" s="30"/>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11" s="28">
@@ -26164,15 +26173,15 @@
         <v>-0.10232203729697265</v>
       </c>
       <c r="I11" s="1"/>
-      <c r="J11" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="K11" s="34"/>
-      <c r="L11" s="35"/>
-      <c r="M11" s="47">
+      <c r="J11" s="43" t="s">
+        <v>11</v>
+      </c>
+      <c r="K11" s="44"/>
+      <c r="L11" s="45"/>
+      <c r="M11" s="30">
         <v>9.9999999999999995E-8</v>
       </c>
-      <c r="N11" s="47"/>
+      <c r="N11" s="30"/>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12" s="28">
@@ -26203,15 +26212,15 @@
         <v>0.16425105273711615</v>
       </c>
       <c r="I12" s="1"/>
-      <c r="J12" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="K12" s="34"/>
-      <c r="L12" s="35"/>
-      <c r="M12" s="47">
+      <c r="J12" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="K12" s="44"/>
+      <c r="L12" s="45"/>
+      <c r="M12" s="30">
         <v>6800000</v>
       </c>
-      <c r="N12" s="47"/>
+      <c r="N12" s="30"/>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A13" s="28">
@@ -26276,16 +26285,16 @@
         <v>-4.6029677160616345E-2</v>
       </c>
       <c r="I14" s="1"/>
-      <c r="J14" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="K14" s="34"/>
-      <c r="L14" s="35"/>
-      <c r="M14" s="47">
+      <c r="J14" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="K14" s="44"/>
+      <c r="L14" s="45"/>
+      <c r="M14" s="30">
         <f>J4</f>
         <v>4134269.0996591127</v>
       </c>
-      <c r="N14" s="47"/>
+      <c r="N14" s="30"/>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A15" s="28">
@@ -26316,11 +26325,11 @@
         <v>0.11054341287347036</v>
       </c>
       <c r="I15" s="1"/>
-      <c r="J15" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="K15" s="34"/>
-      <c r="L15" s="35"/>
+      <c r="J15" s="43" t="s">
+        <v>31</v>
+      </c>
+      <c r="K15" s="44"/>
+      <c r="L15" s="45"/>
       <c r="M15" s="51">
         <f>J5</f>
         <v>56358.769354844706</v>
@@ -26356,16 +26365,16 @@
         <v>-0.12288349709243995</v>
       </c>
       <c r="I16" s="1"/>
-      <c r="J16" s="32" t="s">
-        <v>35</v>
-      </c>
-      <c r="K16" s="32"/>
-      <c r="L16" s="32"/>
-      <c r="M16" s="47">
+      <c r="J16" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="K16" s="48"/>
+      <c r="L16" s="48"/>
+      <c r="M16" s="30">
         <f>F20</f>
         <v>3806771.7273368905</v>
       </c>
-      <c r="N16" s="47"/>
+      <c r="N16" s="30"/>
     </row>
     <row r="17" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="28">
@@ -26397,10 +26406,10 @@
       </c>
       <c r="I17" s="1"/>
       <c r="J17" s="53" t="s">
-        <v>36</v>
-      </c>
-      <c r="K17" s="30"/>
-      <c r="L17" s="30"/>
+        <v>33</v>
+      </c>
+      <c r="K17" s="46"/>
+      <c r="L17" s="46"/>
       <c r="M17" s="51">
         <f>SQRT(((1/D20)*B22)^2+(-(B20/(D20^2))*D22)^2)</f>
         <v>777133.14715069497</v>
@@ -26443,16 +26452,16 @@
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-      <c r="J19" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="K19" s="36"/>
-      <c r="L19" s="36"/>
-      <c r="M19" s="50">
+      <c r="J19" s="50" t="s">
+        <v>17</v>
+      </c>
+      <c r="K19" s="50"/>
+      <c r="L19" s="50"/>
+      <c r="M19" s="42">
         <f>ABS((M12-M14)/M12)</f>
         <v>0.3920192500501305</v>
       </c>
-      <c r="N19" s="50"/>
+      <c r="N19" s="42"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="29" t="s">
@@ -26462,23 +26471,23 @@
         <f>AVERAGE(B4:B18)</f>
         <v>6.2013333333333343</v>
       </c>
-      <c r="C20" s="38"/>
+      <c r="C20" s="34"/>
       <c r="D20" s="19">
         <f>AVERAGE(D4:D18)</f>
         <v>1.5933333333333335E-6</v>
       </c>
-      <c r="E20" s="41"/>
+      <c r="E20" s="37"/>
       <c r="F20" s="19">
         <f>AVERAGE(F4:F18)</f>
         <v>3806771.7273368905</v>
       </c>
-      <c r="G20" s="44"/>
-      <c r="H20" s="44"/>
-      <c r="J20" s="36"/>
-      <c r="K20" s="36"/>
-      <c r="L20" s="36"/>
-      <c r="M20" s="50"/>
-      <c r="N20" s="50"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="40"/>
+      <c r="J20" s="50"/>
+      <c r="K20" s="50"/>
+      <c r="L20" s="50"/>
+      <c r="M20" s="42"/>
+      <c r="N20" s="42"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="29" t="s">
@@ -26488,28 +26497,28 @@
         <f>STDEVA(B4:B18)</f>
         <v>2.8526450549487934</v>
       </c>
-      <c r="C21" s="39"/>
+      <c r="C21" s="35"/>
       <c r="D21" s="19">
         <f>STDEVA(D4:D18)</f>
         <v>6.8916789025054048E-7</v>
       </c>
-      <c r="E21" s="42"/>
+      <c r="E21" s="38"/>
       <c r="F21" s="19">
         <f>STDEVA(F4:F18)</f>
         <v>240042.60206381421</v>
       </c>
-      <c r="G21" s="44"/>
-      <c r="H21" s="44"/>
-      <c r="J21" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="K21" s="31"/>
-      <c r="L21" s="31"/>
-      <c r="M21" s="45">
+      <c r="G21" s="40"/>
+      <c r="H21" s="40"/>
+      <c r="J21" s="46" t="s">
+        <v>20</v>
+      </c>
+      <c r="K21" s="49"/>
+      <c r="L21" s="49"/>
+      <c r="M21" s="41">
         <f>ABS((M12-F20)/M12)</f>
         <v>0.44018062833281024</v>
       </c>
-      <c r="N21" s="45"/>
+      <c r="N21" s="41"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="29" t="s">
@@ -26519,23 +26528,23 @@
         <f>B21/SQRT(10)</f>
         <v>0.90208557296543679</v>
       </c>
-      <c r="C22" s="40"/>
+      <c r="C22" s="36"/>
       <c r="D22" s="19">
         <f>D21/SQRT(10)</f>
         <v>2.1793402234446575E-7</v>
       </c>
-      <c r="E22" s="43"/>
+      <c r="E22" s="39"/>
       <c r="F22" s="19">
         <f t="shared" ref="F22" si="1">F21/SQRT(10)</f>
         <v>75908.135799508775</v>
       </c>
-      <c r="G22" s="44"/>
-      <c r="H22" s="44"/>
-      <c r="J22" s="31"/>
-      <c r="K22" s="31"/>
-      <c r="L22" s="31"/>
-      <c r="M22" s="45"/>
-      <c r="N22" s="45"/>
+      <c r="G22" s="40"/>
+      <c r="H22" s="40"/>
+      <c r="J22" s="49"/>
+      <c r="K22" s="49"/>
+      <c r="L22" s="49"/>
+      <c r="M22" s="41"/>
+      <c r="N22" s="41"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="I27" s="1"/>
@@ -27790,6 +27799,21 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="J15:L15"/>
+    <mergeCell ref="E20:E22"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="G20:H22"/>
+    <mergeCell ref="J14:L14"/>
+    <mergeCell ref="J12:L12"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="J10:L10"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="M15:N15"/>
     <mergeCell ref="M19:N20"/>
     <mergeCell ref="M21:N22"/>
     <mergeCell ref="J16:L16"/>
@@ -27798,21 +27822,6 @@
     <mergeCell ref="M17:N17"/>
     <mergeCell ref="J19:L20"/>
     <mergeCell ref="J21:L22"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="J12:L12"/>
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="J10:L10"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="J15:L15"/>
-    <mergeCell ref="E20:E22"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="G20:H22"/>
-    <mergeCell ref="J14:L14"/>
   </mergeCells>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="9.8425196850393706E-2" bottom="9.8425196850393706E-2" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -27824,18 +27833,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -28009,14 +28018,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF8CA081-A56A-407E-BC39-67D7C2082E3C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60169DA3-410F-42F9-98E4-43875082A5B2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="50696793-6437-4e87-ba7e-0fc4fcfbac97"/>
@@ -28028,6 +28029,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF8CA081-A56A-407E-BC39-67D7C2082E3C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>